<commit_message>
change vlaue and function name, change inner structure
</commit_message>
<xml_diff>
--- a/DOC/재생 적용 HVMT 프로토콜.xlsx
+++ b/DOC/재생 적용 HVMT 프로토콜.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\YJKIM\Documents\Project\14. recycle\DOC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BD292-84EC-43CC-9E37-5C376C2BE2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Can Protocol(HVMT to SAN" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="SAN to HVMT" sheetId="2" r:id="rId5"/>
+    <sheet name="Can Protocol(HVMT to SAN" sheetId="1" r:id="rId1"/>
+    <sheet name="SAN to HVMT" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Fuel_Cell_Idle_Stop_FC_Stop__command_signal__연료전지_시스템_Idle_Stop_FC_Stop__명령_신호">#REF!</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="+0iuPI7A7SLLNnNvSJUzgqFi1IRI+lorFhCRtZ0X9aY="/>
     </ext>
@@ -19,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>CAN_ID</t>
   </si>
@@ -55,39 +74,19 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>0x6N0
-(N : HVMT Number)
-[고전압배터리와 버스전압 모니터링]</t>
-  </si>
-  <si>
-    <t>HVB_CHARGE_RY</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
     <t>0 : OPEN, 1 : CLOSE</t>
   </si>
   <si>
-    <t>HVB_DISCHARGE_RY</t>
-  </si>
-  <si>
-    <t>HVB_PRECHARGE_RY</t>
-  </si>
-  <si>
     <t>Reserved</t>
-  </si>
-  <si>
-    <t>flag</t>
   </si>
   <si>
     <t>HV_AD1_Low byte</t>
   </si>
   <si>
     <t>V</t>
-  </si>
-  <si>
-    <t>Set MaxCurrent</t>
   </si>
   <si>
     <t>HV_AD1_High byte</t>
@@ -97,11 +96,6 @@
   </si>
   <si>
     <t>HV_AD2_High byte</t>
-  </si>
-  <si>
-    <t>0x6N1
-(N : HVMT Number)
-[절연감시장치]</t>
   </si>
   <si>
     <t>relay1</t>
@@ -116,49 +110,54 @@
     <t>relay4</t>
   </si>
   <si>
-    <t>… N 값 만 추가</t>
+    <t>0 : Open, 1 : Close</t>
+  </si>
+  <si>
+    <t>0x6N0
+(N : HVMT Number)
+[Relay 동작상태와 전압 모니터링]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>0x6NA
 (N : HVMT Number)
-[고전압배터리와 절연감시장치 명령]</t>
-  </si>
-  <si>
-    <t>CHARGE</t>
-  </si>
-  <si>
-    <t>0 : None, 1 : Close</t>
-  </si>
-  <si>
-    <t>DISCHARGE</t>
-  </si>
-  <si>
-    <t>0 : Open, 1 : Close</t>
-  </si>
-  <si>
-    <t>…  N 값 만 추가</t>
+[Relay 제어]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
-    <font/>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -167,7 +166,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -182,8 +181,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
-    <border/>
+  <borders count="25">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -197,6 +202,7 @@
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -211,6 +217,7 @@
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -225,6 +232,7 @@
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -234,6 +242,8 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -246,6 +256,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -255,6 +266,8 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,6 +280,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -275,6 +289,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -289,6 +306,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -297,6 +315,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,6 +332,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -322,6 +344,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -330,9 +354,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -341,114 +367,296 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="40">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -638,38 +846,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:L963"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="32.43"/>
-    <col customWidth="1" min="4" max="4" width="8.14"/>
-    <col customWidth="1" min="5" max="5" width="9.14"/>
-    <col customWidth="1" min="6" max="6" width="14.14"/>
-    <col customWidth="1" min="7" max="7" width="7.43"/>
-    <col customWidth="1" min="8" max="9" width="14.14"/>
-    <col customWidth="1" min="10" max="10" width="5.71"/>
-    <col customWidth="1" min="11" max="11" width="9.43"/>
-    <col customWidth="1" min="12" max="12" width="35.71"/>
-    <col customWidth="1" min="13" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" customWidth="1"/>
+    <col min="8" max="9" width="14.08984375" customWidth="1"/>
+    <col min="10" max="10" width="5.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="35.7265625" customWidth="1"/>
+    <col min="13" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1"/>
-    <row r="2" ht="17.25" customHeight="1">
+    <row r="1" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="2" spans="2:12" ht="17.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,499 +912,295 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="17.25" customHeight="1">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="K3" s="17">
+        <v>500</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J3" s="6" t="s">
+    </row>
+    <row r="4" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B4" s="15"/>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" ref="E4:E11" si="0">E3+D3</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B5" s="15"/>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B6" s="15"/>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B7" s="15"/>
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9" t="s">
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B8" s="15"/>
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="9">
+        <v>8</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <v>65535</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="10"/>
     </row>
-    <row r="4" ht="17.25" customHeight="1">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11" t="s">
+    <row r="9" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B9" s="15"/>
+      <c r="C9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B10" s="15"/>
+      <c r="C10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9">
+        <v>8</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="20">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20">
+        <v>65535</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="12">
-        <f t="shared" ref="E4:E13" si="1">E3+D3</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="K10" s="18"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B11" s="15"/>
+      <c r="C11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9">
+        <v>8</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="D12" s="9">
+        <v>32</v>
+      </c>
+      <c r="E12" s="9">
+        <f>E10+D10</f>
+        <v>32</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="12"/>
     </row>
-    <row r="5" ht="17.25" customHeight="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="12">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="9" t="s">
-        <v>14</v>
-      </c>
+    <row r="13" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B13" s="13"/>
     </row>
-    <row r="6" ht="17.25" customHeight="1">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="12">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" ht="17.25" customHeight="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="12">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" ht="17.25" customHeight="1">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="12">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" ht="17.25" customHeight="1">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="E9" s="12">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" ht="17.25" customHeight="1">
-      <c r="B10" s="10"/>
-      <c r="C10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="E10" s="12">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F10" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="G10" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="I10" s="16">
-        <v>65535.0</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" ht="17.25" customHeight="1">
-      <c r="B11" s="10"/>
-      <c r="C11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="E11" s="12">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" ht="17.25" customHeight="1">
-      <c r="B12" s="10"/>
-      <c r="C12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="E12" s="12">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F12" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="16">
-        <v>65535.0</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" ht="17.25" customHeight="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="E13" s="12">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" ht="17.25" customHeight="1">
-      <c r="B14" s="19"/>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="12">
-        <v>32.0</v>
-      </c>
-      <c r="E14" s="12">
-        <f>E12+D12</f>
-        <v>32</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="20"/>
-    </row>
-    <row r="15" ht="17.25" customHeight="1">
-      <c r="B15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" ht="17.25" customHeight="1">
-      <c r="B16" s="10"/>
-      <c r="C16" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="E16" s="12">
-        <f t="shared" ref="E16:E19" si="2">E15+D15</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G16" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I16" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" ht="17.25" customHeight="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="E17" s="12">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G17" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H17" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" ht="17.25" customHeight="1">
-      <c r="B18" s="10"/>
-      <c r="C18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="E18" s="12">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I18" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" ht="17.25" customHeight="1">
-      <c r="B19" s="19"/>
-      <c r="C19" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="23">
-        <v>60.0</v>
-      </c>
-      <c r="E19" s="12">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="14"/>
-    </row>
-    <row r="20" ht="17.25" customHeight="1">
-      <c r="B20" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="14" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="15" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="16" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="17" ht="17.25" customHeight="1"/>
+    <row r="18" ht="17.25" customHeight="1"/>
+    <row r="19" ht="17.25" customHeight="1"/>
+    <row r="20" ht="17.25" customHeight="1"/>
     <row r="21" ht="17.25" customHeight="1"/>
     <row r="22" ht="17.25" customHeight="1"/>
     <row r="23" ht="17.25" customHeight="1"/>
@@ -2140,324 +2144,262 @@
     <row r="961" ht="17.25" customHeight="1"/>
     <row r="962" ht="17.25" customHeight="1"/>
     <row r="963" ht="17.25" customHeight="1"/>
-    <row r="964" ht="17.25" customHeight="1"/>
-    <row r="965" ht="17.25" customHeight="1"/>
-    <row r="966" ht="17.25" customHeight="1"/>
-    <row r="967" ht="17.25" customHeight="1"/>
-    <row r="968" ht="17.25" customHeight="1"/>
-    <row r="969" ht="17.25" customHeight="1"/>
-    <row r="970" ht="17.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B3:B14"/>
-    <mergeCell ref="K3:K14"/>
+  <mergeCells count="12">
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="K3:K12"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="K15:K19"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:L990"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="20.43"/>
-    <col customWidth="1" min="3" max="3" width="29.14"/>
-    <col customWidth="1" min="4" max="4" width="8.14"/>
-    <col customWidth="1" min="5" max="5" width="9.14"/>
-    <col customWidth="1" min="6" max="6" width="7.0"/>
-    <col customWidth="1" min="7" max="7" width="7.43"/>
-    <col customWidth="1" min="8" max="8" width="5.14"/>
-    <col customWidth="1" min="9" max="10" width="8.71"/>
-    <col customWidth="1" min="11" max="11" width="9.71"/>
-    <col customWidth="1" min="12" max="12" width="35.43"/>
-    <col customWidth="1" min="13" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.08984375" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" customWidth="1"/>
+    <col min="8" max="8" width="5.08984375" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="12" max="12" width="35.453125" customWidth="1"/>
+    <col min="13" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1"/>
-    <row r="2" ht="17.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:12" ht="17.25" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:12" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="17.25" customHeight="1">
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J3" s="6" t="s">
+    <row r="3" spans="2:12" ht="17.25" customHeight="1" thickTop="1">
+      <c r="B3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="28">
+        <v>1</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0</v>
+      </c>
+      <c r="F3" s="28">
+        <v>0</v>
+      </c>
+      <c r="G3" s="28">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28">
+        <v>0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="29">
+        <v>500</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B4" s="31"/>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" ref="E4:E7" si="0">E3+D3</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="28">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28">
+        <v>1</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0</v>
+      </c>
+      <c r="I4" s="28">
+        <v>1</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B5" s="31"/>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0</v>
+      </c>
+      <c r="G5" s="28">
+        <v>1</v>
+      </c>
+      <c r="H5" s="28">
+        <v>0</v>
+      </c>
+      <c r="I5" s="28">
+        <v>1</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B6" s="31"/>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>1</v>
+      </c>
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>1</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9" t="s">
-        <v>33</v>
+      <c r="D7" s="35">
+        <v>60</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="36">
+        <v>0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>1</v>
+      </c>
+      <c r="H7" s="36">
+        <v>0</v>
+      </c>
+      <c r="I7" s="36">
+        <v>1</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" ht="17.25" customHeight="1">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="12">
-        <f t="shared" ref="E4:E9" si="1">E3+D3</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="9" t="s">
-        <v>33</v>
-      </c>
+    <row r="8" spans="2:12" ht="17.25" customHeight="1">
+      <c r="B8" s="13"/>
     </row>
-    <row r="5" ht="17.25" customHeight="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="12">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" ht="17.25" customHeight="1">
-      <c r="B6" s="10"/>
-      <c r="C6" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="12">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" ht="17.25" customHeight="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="12">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" ht="17.25" customHeight="1">
-      <c r="B8" s="10"/>
-      <c r="C8" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="12">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" ht="17.25" customHeight="1">
-      <c r="B9" s="19"/>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="12">
-        <v>58.0</v>
-      </c>
-      <c r="E9" s="12">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" ht="17.25" customHeight="1">
-      <c r="B10" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" ht="17.25" customHeight="1"/>
-    <row r="12" ht="17.25" customHeight="1"/>
-    <row r="13" ht="17.25" customHeight="1"/>
-    <row r="14" ht="17.25" customHeight="1"/>
-    <row r="15" ht="17.25" customHeight="1"/>
-    <row r="16" ht="17.25" customHeight="1"/>
+    <row r="9" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="10" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="11" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="12" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="13" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="14" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="15" spans="2:12" ht="17.25" customHeight="1"/>
+    <row r="16" spans="2:12" ht="17.25" customHeight="1"/>
     <row r="17" ht="17.25" customHeight="1"/>
     <row r="18" ht="17.25" customHeight="1"/>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -3432,16 +3374,13 @@
     <row r="988" ht="17.25" customHeight="1"/>
     <row r="989" ht="17.25" customHeight="1"/>
     <row r="990" ht="17.25" customHeight="1"/>
-    <row r="991" ht="17.25" customHeight="1"/>
-    <row r="992" ht="17.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="K3:K9"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="K3:K7"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>